<commit_message>
Update Method to update compliance_groups
Signed-off-by: el harag <elharag@cyberwatch.fr>
</commit_message>
<xml_diff>
--- a/examples/import_file.xlsx
+++ b/examples/import_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t xml:space="preserve">HOST</t>
   </si>
@@ -34,16 +34,19 @@
     <t xml:space="preserve">NODE</t>
   </si>
   <si>
+    <t xml:space="preserve">KEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USERNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASSWORD</t>
+  </si>
+  <si>
     <t xml:space="preserve">GROUPS</t>
   </si>
   <si>
-    <t xml:space="preserve">USERNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PASSWORD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KEY</t>
+    <t xml:space="preserve">COMPLIANCE_GROUPS</t>
   </si>
   <si>
     <t xml:space="preserve">server01.example.com</t>
@@ -55,19 +58,19 @@
     <t xml:space="preserve">master</t>
   </si>
   <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SuperPassword</t>
+  </si>
+  <si>
     <t xml:space="preserve">production, test</t>
   </si>
   <si>
-    <t xml:space="preserve">admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SuperPassword</t>
+    <t xml:space="preserve">Anssi</t>
   </si>
   <si>
     <t xml:space="preserve">server02.example.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user</t>
   </si>
   <si>
     <t xml:space="preserve">---- BEGIN SSH2 PUBLIC KEY ----
@@ -84,6 +87,9 @@
 ---- END SSH2 PUBLIC KEY ----</t>
   </si>
   <si>
+    <t xml:space="preserve">user</t>
+  </si>
+  <si>
     <t xml:space="preserve">127.0.0.1</t>
   </si>
   <si>
@@ -93,13 +99,13 @@
     <t xml:space="preserve">slave1</t>
   </si>
   <si>
+    <t xml:space="preserve">Administrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nu6K2WBX</t>
+  </si>
+  <si>
     <t xml:space="preserve">preproduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Administrator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nu6K2WBX</t>
   </si>
 </sst>
 </file>
@@ -109,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -131,6 +137,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -175,13 +187,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -205,10 +225,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -216,7 +236,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -238,74 +258,88 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
+      <c r="A2" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>22</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="1310.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>22</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>5985</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated examples to use remote_access method with server_groups
</commit_message>
<xml_diff>
--- a/examples/import_file.xlsx
+++ b/examples/import_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t xml:space="preserve">HOST</t>
   </si>
@@ -43,10 +43,7 @@
     <t xml:space="preserve">PASSWORD</t>
   </si>
   <si>
-    <t xml:space="preserve">GROUPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMPLIANCE_GROUPS</t>
+    <t xml:space="preserve">SERVER_GROUPS</t>
   </si>
   <si>
     <t xml:space="preserve">server01.example.com</t>
@@ -65,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">production, test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anssi</t>
   </si>
   <si>
     <t xml:space="preserve">server02.example.com</t>
@@ -115,7 +109,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -137,12 +131,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -187,21 +175,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -225,13 +205,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
   </cols>
@@ -261,85 +241,73 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
+      <c r="A2" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>22</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="1303.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>16</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>22</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>5985</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>